<commit_message>
Warning message for Labor Area
- added warning message when selecting labor area
</commit_message>
<xml_diff>
--- a/Translation sheets/TranslationForm.xlsx
+++ b/Translation sheets/TranslationForm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Repository\Prison Labor Mod\Translation sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3010D0F-9A86-43CA-9282-3D1470E8B410}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6219301A-909A-49DB-93E0-1F65D8659E94}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8820" xr2:uid="{CF5D6EBD-60F8-43F9-A1CC-353B0616DA62}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="228">
   <si>
     <t>English</t>
   </si>
@@ -731,6 +731,36 @@
   </si>
   <si>
     <t>XML Value</t>
+  </si>
+  <si>
+    <t>PrisonLabor_EnableRevolts</t>
+  </si>
+  <si>
+    <t>PrisonLabor_EnableRevoltsDesc</t>
+  </si>
+  <si>
+    <t>PrisonLabor_LaborAreaWarning</t>
+  </si>
+  <si>
+    <t>PrisonLabor_DontShowAgain</t>
+  </si>
+  <si>
+    <t>Enable revolts</t>
+  </si>
+  <si>
+    <t>When enabled revolts will sometimes occur instead of vanilla incidents</t>
+  </si>
+  <si>
+    <t>Labor area isn't required to make prisoners work.\n\nThis area forbids colonists from working.\n\nIt's for situations where you don't want colonists to work in certain area. Prisoners will work anywhere they can enter.</t>
+  </si>
+  <si>
+    <t>Don't show again</t>
+  </si>
+  <si>
+    <t>warining message when clicking labor area</t>
+  </si>
+  <si>
+    <t>button on warning message box</t>
   </si>
 </sst>
 </file>
@@ -1170,7 +1200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1300,6 +1330,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1580,8 +1623,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E789CC9E-5DB3-44D7-B3BF-A6DB59D858C3}" name="Tabela1" displayName="Tabela1" ref="I2:K101" tableType="xml" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3" connectionId="5">
-  <autoFilter ref="I2:K101" xr:uid="{A0B2254A-B303-4A68-A399-8E0730B7AE6D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E789CC9E-5DB3-44D7-B3BF-A6DB59D858C3}" name="Tabela1" displayName="Tabela1" ref="I2:K105" tableType="xml" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3" connectionId="5">
+  <autoFilter ref="I2:K105" xr:uid="{A0B2254A-B303-4A68-A399-8E0730B7AE6D}"/>
   <tableColumns count="3">
     <tableColumn id="2" xr3:uid="{1779611B-9B22-4127-BE9E-F389F3211919}" uniqueName="document" name="XML Document" dataDxfId="2">
       <calculatedColumnFormula>H$2</calculatedColumnFormula>
@@ -1898,10 +1941,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7B04E6-7593-465F-8DFF-3C928DB22BF4}">
   <sheetPr codeName="Arkusz1"/>
-  <dimension ref="A1:Q321"/>
+  <dimension ref="A1:Q325"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="C43" workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3425,14 +3468,14 @@
         <v>214</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="9" t="s">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="C47" s="35"/>
+      <c r="C47" s="64"/>
       <c r="D47" s="12" t="s">
         <v>214</v>
       </c>
@@ -3458,158 +3501,150 @@
         <v>214</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="B48" s="55"/>
-      <c r="C48" s="55"/>
-      <c r="D48" s="12" t="s">
-        <v>214</v>
-      </c>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C48" s="34"/>
+      <c r="D48" s="12"/>
       <c r="E48" s="11"/>
       <c r="F48" s="11"/>
       <c r="G48" s="11"/>
-      <c r="H48" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="I48" s="42"/>
-      <c r="J48" s="43"/>
-      <c r="K48" s="48"/>
-      <c r="L48" s="20" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="8"/>
-      <c r="B49" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C49" s="33"/>
-      <c r="D49" s="12" t="s">
-        <v>214</v>
-      </c>
+      <c r="H48" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="I48" s="44" t="str">
+        <f>H$2</f>
+        <v>Keyed\Keys.xml</v>
+      </c>
+      <c r="J48" s="26" t="str">
+        <f>H48</f>
+        <v>PrisonLabor_EnableRevolts</v>
+      </c>
+      <c r="K48" s="61" t="str">
+        <f>C48&amp;""</f>
+        <v/>
+      </c>
+      <c r="L48" s="20"/>
+    </row>
+    <row r="49" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C49" s="34"/>
+      <c r="D49" s="12"/>
       <c r="E49" s="11"/>
       <c r="F49" s="11"/>
       <c r="G49" s="11"/>
       <c r="H49" s="13" t="s">
-        <v>161</v>
+        <v>219</v>
       </c>
       <c r="I49" s="44" t="str">
-        <f t="shared" ref="I49:I58" si="3">H$48</f>
-        <v>DefInjected\ConceptDef\ConceptDef.xml</v>
-      </c>
-      <c r="J49" s="41" t="str">
-        <f t="shared" ref="J49:J58" si="4">H49</f>
-        <v>PrisonLabor_Indroduction.label</v>
-      </c>
-      <c r="K49" s="47" t="str">
-        <f t="shared" ref="K49:K58" si="5">C49&amp;""</f>
-        <v/>
-      </c>
-      <c r="L49" s="20" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" ht="150" x14ac:dyDescent="0.25">
-      <c r="A50" s="9"/>
-      <c r="B50" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C50" s="34"/>
-      <c r="D50" s="12" t="s">
-        <v>214</v>
-      </c>
+        <f>H$2</f>
+        <v>Keyed\Keys.xml</v>
+      </c>
+      <c r="J49" s="26" t="str">
+        <f>H49</f>
+        <v>PrisonLabor_EnableRevoltsDesc</v>
+      </c>
+      <c r="K49" s="61" t="str">
+        <f>C49&amp;""</f>
+        <v/>
+      </c>
+      <c r="L49" s="20"/>
+    </row>
+    <row r="50" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C50" s="33"/>
+      <c r="D50" s="12"/>
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
       <c r="G50" s="11"/>
       <c r="H50" s="13" t="s">
-        <v>162</v>
+        <v>220</v>
       </c>
       <c r="I50" s="44" t="str">
-        <f t="shared" si="3"/>
-        <v>DefInjected\ConceptDef\ConceptDef.xml</v>
-      </c>
-      <c r="J50" s="41" t="str">
-        <f t="shared" si="4"/>
-        <v>PrisonLabor_Indroduction.helpText</v>
-      </c>
-      <c r="K50" s="47" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="L50" s="20" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="9"/>
-      <c r="B51" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C51" s="34"/>
-      <c r="D51" s="12" t="s">
-        <v>214</v>
-      </c>
+        <f>H$2</f>
+        <v>Keyed\Keys.xml</v>
+      </c>
+      <c r="J50" s="26" t="str">
+        <f>H50</f>
+        <v>PrisonLabor_LaborAreaWarning</v>
+      </c>
+      <c r="K50" s="61" t="str">
+        <f>C50&amp;""</f>
+        <v/>
+      </c>
+      <c r="L50" s="20"/>
+    </row>
+    <row r="51" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="C51" s="60"/>
+      <c r="D51" s="12"/>
       <c r="E51" s="11"/>
       <c r="F51" s="11"/>
       <c r="G51" s="11"/>
       <c r="H51" s="13" t="s">
-        <v>163</v>
+        <v>221</v>
       </c>
       <c r="I51" s="44" t="str">
-        <f t="shared" si="3"/>
-        <v>DefInjected\ConceptDef\ConceptDef.xml</v>
-      </c>
-      <c r="J51" s="41" t="str">
-        <f t="shared" si="4"/>
-        <v>PrisonLabor_Motivation.label</v>
-      </c>
-      <c r="K51" s="47" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="L51" s="20" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A52" s="9"/>
-      <c r="B52" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C52" s="34"/>
+        <f>H$2</f>
+        <v>Keyed\Keys.xml</v>
+      </c>
+      <c r="J51" s="26" t="str">
+        <f>H51</f>
+        <v>PrisonLabor_DontShowAgain</v>
+      </c>
+      <c r="K51" s="61" t="str">
+        <f>C51&amp;""</f>
+        <v/>
+      </c>
+      <c r="L51" s="20"/>
+    </row>
+    <row r="52" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="B52" s="55"/>
+      <c r="C52" s="55"/>
       <c r="D52" s="12" t="s">
         <v>214</v>
       </c>
       <c r="E52" s="11"/>
       <c r="F52" s="11"/>
       <c r="G52" s="11"/>
-      <c r="H52" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="I52" s="44" t="str">
-        <f t="shared" si="3"/>
-        <v>DefInjected\ConceptDef\ConceptDef.xml</v>
-      </c>
-      <c r="J52" s="41" t="str">
-        <f t="shared" si="4"/>
-        <v>PrisonLabor_Motivation.helpText</v>
-      </c>
-      <c r="K52" s="47" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="H52" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="I52" s="42"/>
+      <c r="J52" s="43"/>
+      <c r="K52" s="48"/>
       <c r="L52" s="20" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="9"/>
-      <c r="B53" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C53" s="34"/>
+      <c r="A53" s="8"/>
+      <c r="B53" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C53" s="33"/>
       <c r="D53" s="12" t="s">
         <v>214</v>
       </c>
@@ -3617,28 +3652,28 @@
       <c r="F53" s="11"/>
       <c r="G53" s="11"/>
       <c r="H53" s="13" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="I53" s="44" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="I53:I62" si="3">H$52</f>
         <v>DefInjected\ConceptDef\ConceptDef.xml</v>
       </c>
       <c r="J53" s="41" t="str">
-        <f t="shared" si="4"/>
-        <v>PrisonLabor_Growing.label</v>
+        <f t="shared" ref="J53:J62" si="4">H53</f>
+        <v>PrisonLabor_Indroduction.label</v>
       </c>
       <c r="K53" s="47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="K53:K62" si="5">C53&amp;""</f>
         <v/>
       </c>
       <c r="L53" s="20" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
       <c r="B54" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C54" s="34"/>
       <c r="D54" s="12" t="s">
@@ -3648,7 +3683,7 @@
       <c r="F54" s="11"/>
       <c r="G54" s="11"/>
       <c r="H54" s="13" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="I54" s="44" t="str">
         <f t="shared" si="3"/>
@@ -3656,7 +3691,7 @@
       </c>
       <c r="J54" s="41" t="str">
         <f t="shared" si="4"/>
-        <v>PrisonLabor_Growing.helpText</v>
+        <v>PrisonLabor_Indroduction.helpText</v>
       </c>
       <c r="K54" s="47" t="str">
         <f t="shared" si="5"/>
@@ -3669,7 +3704,7 @@
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="9"/>
       <c r="B55" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C55" s="34"/>
       <c r="D55" s="12" t="s">
@@ -3679,7 +3714,7 @@
       <c r="F55" s="11"/>
       <c r="G55" s="11"/>
       <c r="H55" s="13" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="I55" s="44" t="str">
         <f t="shared" si="3"/>
@@ -3687,7 +3722,7 @@
       </c>
       <c r="J55" s="41" t="str">
         <f t="shared" si="4"/>
-        <v>PrisonLabor_Management.label</v>
+        <v>PrisonLabor_Motivation.label</v>
       </c>
       <c r="K55" s="47" t="str">
         <f t="shared" si="5"/>
@@ -3697,10 +3732,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
       <c r="B56" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C56" s="34"/>
       <c r="D56" s="12" t="s">
@@ -3710,7 +3745,7 @@
       <c r="F56" s="11"/>
       <c r="G56" s="11"/>
       <c r="H56" s="13" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="I56" s="44" t="str">
         <f t="shared" si="3"/>
@@ -3718,7 +3753,7 @@
       </c>
       <c r="J56" s="41" t="str">
         <f t="shared" si="4"/>
-        <v>PrisonLabor_Management.helpText</v>
+        <v>PrisonLabor_Motivation.helpText</v>
       </c>
       <c r="K56" s="47" t="str">
         <f t="shared" si="5"/>
@@ -3731,7 +3766,7 @@
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="9"/>
       <c r="B57" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C57" s="34"/>
       <c r="D57" s="12" t="s">
@@ -3741,7 +3776,7 @@
       <c r="F57" s="11"/>
       <c r="G57" s="11"/>
       <c r="H57" s="13" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="I57" s="44" t="str">
         <f t="shared" si="3"/>
@@ -3749,7 +3784,7 @@
       </c>
       <c r="J57" s="41" t="str">
         <f t="shared" si="4"/>
-        <v>PrisonLabor_Timetable.label</v>
+        <v>PrisonLabor_Growing.label</v>
       </c>
       <c r="K57" s="47" t="str">
         <f t="shared" si="5"/>
@@ -3759,12 +3794,12 @@
         <v>214</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="10"/>
-      <c r="B58" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C58" s="35"/>
+    <row r="58" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="9"/>
+      <c r="B58" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C58" s="34"/>
       <c r="D58" s="12" t="s">
         <v>214</v>
       </c>
@@ -3772,7 +3807,7 @@
       <c r="F58" s="11"/>
       <c r="G58" s="11"/>
       <c r="H58" s="13" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="I58" s="44" t="str">
         <f t="shared" si="3"/>
@@ -3780,7 +3815,7 @@
       </c>
       <c r="J58" s="41" t="str">
         <f t="shared" si="4"/>
-        <v>PrisonLabor_Timetable.helpText</v>
+        <v>PrisonLabor_Growing.helpText</v>
       </c>
       <c r="K58" s="47" t="str">
         <f t="shared" si="5"/>
@@ -3790,34 +3825,43 @@
         <v>214</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="B59" s="55"/>
-      <c r="C59" s="55"/>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="9"/>
+      <c r="B59" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C59" s="34"/>
       <c r="D59" s="12" t="s">
         <v>214</v>
       </c>
       <c r="E59" s="11"/>
       <c r="F59" s="11"/>
       <c r="G59" s="11"/>
-      <c r="H59" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="I59" s="42"/>
-      <c r="J59" s="43"/>
-      <c r="K59" s="48"/>
+      <c r="H59" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="I59" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v>DefInjected\ConceptDef\ConceptDef.xml</v>
+      </c>
+      <c r="J59" s="41" t="str">
+        <f t="shared" si="4"/>
+        <v>PrisonLabor_Management.label</v>
+      </c>
+      <c r="K59" s="47" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="L59" s="20" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="8"/>
-      <c r="B60" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C60" s="33"/>
+    <row r="60" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A60" s="9"/>
+      <c r="B60" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C60" s="34"/>
       <c r="D60" s="12" t="s">
         <v>214</v>
       </c>
@@ -3825,30 +3869,30 @@
       <c r="F60" s="11"/>
       <c r="G60" s="11"/>
       <c r="H60" s="13" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="I60" s="44" t="str">
-        <f>H$59</f>
-        <v>DefInjected\NeedDef\Needs.xml</v>
+        <f t="shared" si="3"/>
+        <v>DefInjected\ConceptDef\ConceptDef.xml</v>
       </c>
       <c r="J60" s="41" t="str">
-        <f>H60</f>
-        <v>PrisonLabor_Motivation.label</v>
+        <f t="shared" si="4"/>
+        <v>PrisonLabor_Management.helpText</v>
       </c>
       <c r="K60" s="47" t="str">
-        <f>C60&amp;""</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="L60" s="20" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="10"/>
-      <c r="B61" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C61" s="35"/>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="9"/>
+      <c r="B61" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C61" s="34"/>
       <c r="D61" s="12" t="s">
         <v>214</v>
       </c>
@@ -3856,88 +3900,83 @@
       <c r="F61" s="11"/>
       <c r="G61" s="11"/>
       <c r="H61" s="13" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I61" s="44" t="str">
-        <f>H$59</f>
-        <v>DefInjected\NeedDef\Needs.xml</v>
+        <f t="shared" si="3"/>
+        <v>DefInjected\ConceptDef\ConceptDef.xml</v>
       </c>
       <c r="J61" s="41" t="str">
-        <f>H61</f>
-        <v>PrisonLabor_Motivation.description</v>
+        <f t="shared" si="4"/>
+        <v>PrisonLabor_Timetable.label</v>
       </c>
       <c r="K61" s="47" t="str">
-        <f>C61&amp;""</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="L61" s="20" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="55" t="s">
-        <v>104</v>
-      </c>
-      <c r="B62" s="55"/>
-      <c r="C62" s="55"/>
+    <row r="62" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="10"/>
+      <c r="B62" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C62" s="35"/>
       <c r="D62" s="12" t="s">
         <v>214</v>
       </c>
       <c r="E62" s="11"/>
       <c r="F62" s="11"/>
       <c r="G62" s="11"/>
-      <c r="H62" s="21" t="s">
-        <v>173</v>
-      </c>
-      <c r="I62" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="J62" s="41"/>
+      <c r="H62" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="I62" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v>DefInjected\ConceptDef\ConceptDef.xml</v>
+      </c>
+      <c r="J62" s="41" t="str">
+        <f t="shared" si="4"/>
+        <v>PrisonLabor_Timetable.helpText</v>
+      </c>
       <c r="K62" s="47" t="str">
-        <f>C62&amp;""</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="L62" s="20" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" s="8"/>
-      <c r="B63" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C63" s="33"/>
+    <row r="63" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="B63" s="55"/>
+      <c r="C63" s="55"/>
       <c r="D63" s="12" t="s">
         <v>214</v>
       </c>
       <c r="E63" s="11"/>
       <c r="F63" s="11"/>
       <c r="G63" s="11"/>
-      <c r="H63" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="I63" s="44" t="str">
-        <f>H$62</f>
-        <v>DefInjected\HediffDef\Hediffs.xml</v>
-      </c>
-      <c r="J63" s="41" t="str">
-        <f>H63</f>
-        <v>PrisonLabor_PrisonerChains.stages.0.label</v>
-      </c>
-      <c r="K63" s="47" t="str">
-        <f>C63&amp;""</f>
-        <v/>
-      </c>
+      <c r="H63" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="I63" s="42"/>
+      <c r="J63" s="43"/>
+      <c r="K63" s="48"/>
       <c r="L63" s="20" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A64" s="9"/>
-      <c r="B64" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C64" s="34"/>
+      <c r="A64" s="8"/>
+      <c r="B64" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C64" s="33"/>
       <c r="D64" s="12" t="s">
         <v>214</v>
       </c>
@@ -3945,15 +3984,15 @@
       <c r="F64" s="11"/>
       <c r="G64" s="11"/>
       <c r="H64" s="13" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="I64" s="44" t="str">
-        <f>H$62</f>
-        <v>DefInjected\HediffDef\Hediffs.xml</v>
+        <f>H$63</f>
+        <v>DefInjected\NeedDef\Needs.xml</v>
       </c>
       <c r="J64" s="41" t="str">
         <f>H64</f>
-        <v>PrisonLabor_PrisonerChains.stages.1.label</v>
+        <v>PrisonLabor_Motivation.label</v>
       </c>
       <c r="K64" s="47" t="str">
         <f>C64&amp;""</f>
@@ -3963,66 +4002,88 @@
         <v>214</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A65" s="9"/>
-      <c r="B65" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C65" s="34"/>
+    <row r="65" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="10"/>
+      <c r="B65" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C65" s="35"/>
       <c r="D65" s="12" t="s">
         <v>214</v>
       </c>
       <c r="E65" s="11"/>
       <c r="F65" s="11"/>
       <c r="G65" s="11"/>
-      <c r="H65" s="13"/>
-      <c r="I65" s="44"/>
-      <c r="J65" s="41"/>
-      <c r="K65" s="47"/>
+      <c r="H65" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="I65" s="44" t="str">
+        <f>H$63</f>
+        <v>DefInjected\NeedDef\Needs.xml</v>
+      </c>
+      <c r="J65" s="41" t="str">
+        <f>H65</f>
+        <v>PrisonLabor_Motivation.description</v>
+      </c>
+      <c r="K65" s="47" t="str">
+        <f>C65&amp;""</f>
+        <v/>
+      </c>
       <c r="L65" s="20" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="10"/>
-      <c r="B66" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C66" s="35"/>
+    <row r="66" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="55" t="s">
+        <v>104</v>
+      </c>
+      <c r="B66" s="55"/>
+      <c r="C66" s="55"/>
       <c r="D66" s="12" t="s">
         <v>214</v>
       </c>
       <c r="E66" s="11"/>
       <c r="F66" s="11"/>
       <c r="G66" s="11"/>
-      <c r="H66" s="13"/>
-      <c r="I66" s="44"/>
+      <c r="H66" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="I66" s="44" t="s">
+        <v>159</v>
+      </c>
       <c r="J66" s="41"/>
-      <c r="K66" s="47"/>
+      <c r="K66" s="47" t="str">
+        <f>C66&amp;""</f>
+        <v/>
+      </c>
       <c r="L66" s="20" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="55" t="s">
-        <v>65</v>
-      </c>
-      <c r="B67" s="55"/>
-      <c r="C67" s="55"/>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" s="8"/>
+      <c r="B67" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C67" s="33"/>
       <c r="D67" s="12" t="s">
         <v>214</v>
       </c>
       <c r="E67" s="11"/>
       <c r="F67" s="11"/>
       <c r="G67" s="11"/>
-      <c r="H67" s="21" t="s">
-        <v>205</v>
-      </c>
-      <c r="I67" s="42" t="s">
-        <v>159</v>
-      </c>
-      <c r="J67" s="43"/>
-      <c r="K67" s="48" t="str">
+      <c r="H67" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="I67" s="44" t="str">
+        <f>H$66</f>
+        <v>DefInjected\HediffDef\Hediffs.xml</v>
+      </c>
+      <c r="J67" s="41" t="str">
+        <f>H67</f>
+        <v>PrisonLabor_PrisonerChains.stages.0.label</v>
+      </c>
+      <c r="K67" s="47" t="str">
         <f>C67&amp;""</f>
         <v/>
       </c>
@@ -4031,11 +4092,11 @@
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A68" s="8"/>
-      <c r="B68" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C68" s="33"/>
+      <c r="A68" s="9"/>
+      <c r="B68" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C68" s="34"/>
       <c r="D68" s="12" t="s">
         <v>214</v>
       </c>
@@ -4043,18 +4104,18 @@
       <c r="F68" s="11"/>
       <c r="G68" s="11"/>
       <c r="H68" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I68" s="44" t="str">
-        <f>H$67</f>
-        <v>DefInjected\IncidentDef\Incidents.xml</v>
+        <f>H$66</f>
+        <v>DefInjected\HediffDef\Hediffs.xml</v>
       </c>
       <c r="J68" s="41" t="str">
-        <f t="shared" ref="J68:J101" si="6">H68</f>
-        <v>PrisonLabor_Revolt.label</v>
+        <f>H68</f>
+        <v>PrisonLabor_PrisonerChains.stages.1.label</v>
       </c>
       <c r="K68" s="47" t="str">
-        <f t="shared" ref="K68:K102" si="7">C68&amp;""</f>
+        <f>C68&amp;""</f>
         <v/>
       </c>
       <c r="L68" s="20" t="s">
@@ -4064,7 +4125,7 @@
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="9"/>
       <c r="B69" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C69" s="34"/>
       <c r="D69" s="12" t="s">
@@ -4073,29 +4134,18 @@
       <c r="E69" s="11"/>
       <c r="F69" s="11"/>
       <c r="G69" s="11"/>
-      <c r="H69" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="I69" s="44" t="str">
-        <f>H$67</f>
-        <v>DefInjected\IncidentDef\Incidents.xml</v>
-      </c>
-      <c r="J69" s="41" t="str">
-        <f t="shared" si="6"/>
-        <v>PrisonLabor_Revolt.letterLabel</v>
-      </c>
-      <c r="K69" s="47" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
+      <c r="H69" s="13"/>
+      <c r="I69" s="44"/>
+      <c r="J69" s="41"/>
+      <c r="K69" s="47"/>
       <c r="L69" s="20" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="10"/>
       <c r="B70" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C70" s="35"/>
       <c r="D70" s="12" t="s">
@@ -4105,9 +4155,7 @@
       <c r="F70" s="11"/>
       <c r="G70" s="11"/>
       <c r="H70" s="13"/>
-      <c r="I70" s="44" t="s">
-        <v>159</v>
-      </c>
+      <c r="I70" s="44"/>
       <c r="J70" s="41"/>
       <c r="K70" s="47"/>
       <c r="L70" s="20" t="s">
@@ -4116,7 +4164,7 @@
     </row>
     <row r="71" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="55" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B71" s="55"/>
       <c r="C71" s="55"/>
@@ -4127,11 +4175,16 @@
       <c r="F71" s="11"/>
       <c r="G71" s="11"/>
       <c r="H71" s="21" t="s">
-        <v>206</v>
-      </c>
-      <c r="I71" s="42"/>
+        <v>205</v>
+      </c>
+      <c r="I71" s="42" t="s">
+        <v>159</v>
+      </c>
       <c r="J71" s="43"/>
-      <c r="K71" s="48"/>
+      <c r="K71" s="48" t="str">
+        <f>C71&amp;""</f>
+        <v/>
+      </c>
       <c r="L71" s="20" t="s">
         <v>214</v>
       </c>
@@ -4139,7 +4192,7 @@
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="8"/>
       <c r="B72" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C72" s="33"/>
       <c r="D72" s="12" t="s">
@@ -4149,18 +4202,18 @@
       <c r="F72" s="11"/>
       <c r="G72" s="11"/>
       <c r="H72" s="13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I72" s="44" t="str">
         <f>H$71</f>
-        <v>DefInjected\JobDef\JobDef.xml</v>
+        <v>DefInjected\IncidentDef\Incidents.xml</v>
       </c>
       <c r="J72" s="41" t="str">
-        <f t="shared" si="6"/>
-        <v>PrisonLabor_PrisonerSupervise.reportString</v>
+        <f t="shared" ref="J72:J105" si="6">H72</f>
+        <v>PrisonLabor_Revolt.label</v>
       </c>
       <c r="K72" s="47" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="K72:K106" si="7">C72&amp;""</f>
         <v/>
       </c>
       <c r="L72" s="20" t="s">
@@ -4168,11 +4221,9 @@
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A73" s="9" t="s">
-        <v>105</v>
-      </c>
+      <c r="A73" s="9"/>
       <c r="B73" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C73" s="34"/>
       <c r="D73" s="12" t="s">
@@ -4182,15 +4233,15 @@
       <c r="F73" s="11"/>
       <c r="G73" s="11"/>
       <c r="H73" s="13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I73" s="44" t="str">
         <f>H$71</f>
-        <v>DefInjected\JobDef\JobDef.xml</v>
+        <v>DefInjected\IncidentDef\Incidents.xml</v>
       </c>
       <c r="J73" s="41" t="str">
         <f t="shared" si="6"/>
-        <v>PrisonLabor_DeliverFood_Tweak.reportString</v>
+        <v>PrisonLabor_Revolt.letterLabel</v>
       </c>
       <c r="K73" s="47" t="str">
         <f t="shared" si="7"/>
@@ -4200,80 +4251,56 @@
         <v>214</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A74" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C74" s="34"/>
+    <row r="74" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="10"/>
+      <c r="B74" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C74" s="35"/>
       <c r="D74" s="12" t="s">
         <v>214</v>
       </c>
       <c r="E74" s="11"/>
       <c r="F74" s="11"/>
       <c r="G74" s="11"/>
-      <c r="H74" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="I74" s="44" t="str">
-        <f>H$71</f>
-        <v>DefInjected\JobDef\JobDef.xml</v>
-      </c>
-      <c r="J74" s="41" t="str">
-        <f t="shared" si="6"/>
-        <v>PrisonLabor_Mine_Tweak.reportString</v>
-      </c>
-      <c r="K74" s="47" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
+      <c r="H74" s="13"/>
+      <c r="I74" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="J74" s="41"/>
+      <c r="K74" s="47"/>
       <c r="L74" s="20" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A75" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C75" s="34"/>
+    <row r="75" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="B75" s="55"/>
+      <c r="C75" s="55"/>
       <c r="D75" s="12" t="s">
         <v>214</v>
       </c>
       <c r="E75" s="11"/>
       <c r="F75" s="11"/>
       <c r="G75" s="11"/>
-      <c r="H75" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="I75" s="44" t="str">
-        <f>H$71</f>
-        <v>DefInjected\JobDef\JobDef.xml</v>
-      </c>
-      <c r="J75" s="41" t="str">
-        <f t="shared" si="6"/>
-        <v>PrisonLabor_Harvest_Tweak.reportString</v>
-      </c>
-      <c r="K75" s="47" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
+      <c r="H75" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="I75" s="42"/>
+      <c r="J75" s="43"/>
+      <c r="K75" s="48"/>
       <c r="L75" s="20" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C76" s="35"/>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" s="8"/>
+      <c r="B76" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C76" s="33"/>
       <c r="D76" s="12" t="s">
         <v>214</v>
       </c>
@@ -4281,15 +4308,15 @@
       <c r="F76" s="11"/>
       <c r="G76" s="11"/>
       <c r="H76" s="13" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="I76" s="44" t="str">
-        <f>H$71</f>
+        <f>H$75</f>
         <v>DefInjected\JobDef\JobDef.xml</v>
       </c>
       <c r="J76" s="41" t="str">
         <f t="shared" si="6"/>
-        <v>PrisonLabor_CutPlant_Tweak.reportString</v>
+        <v>PrisonLabor_PrisonerSupervise.reportString</v>
       </c>
       <c r="K76" s="47" t="str">
         <f t="shared" si="7"/>
@@ -4299,34 +4326,47 @@
         <v>214</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="55" t="s">
-        <v>75</v>
-      </c>
-      <c r="B77" s="55"/>
-      <c r="C77" s="55"/>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C77" s="34"/>
       <c r="D77" s="12" t="s">
         <v>214</v>
       </c>
       <c r="E77" s="11"/>
       <c r="F77" s="11"/>
       <c r="G77" s="11"/>
-      <c r="H77" s="22" t="s">
-        <v>204</v>
-      </c>
-      <c r="I77" s="42"/>
-      <c r="J77" s="43"/>
-      <c r="K77" s="48"/>
+      <c r="H77" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="I77" s="44" t="str">
+        <f>H$75</f>
+        <v>DefInjected\JobDef\JobDef.xml</v>
+      </c>
+      <c r="J77" s="41" t="str">
+        <f t="shared" si="6"/>
+        <v>PrisonLabor_DeliverFood_Tweak.reportString</v>
+      </c>
+      <c r="K77" s="47" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="L77" s="20" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A78" s="8"/>
-      <c r="B78" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C78" s="33"/>
+      <c r="A78" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C78" s="34"/>
       <c r="D78" s="12" t="s">
         <v>214</v>
       </c>
@@ -4334,15 +4374,15 @@
       <c r="F78" s="11"/>
       <c r="G78" s="11"/>
       <c r="H78" s="13" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I78" s="44" t="str">
-        <f t="shared" ref="I78:I98" si="8">H$77</f>
-        <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
+        <f>H$75</f>
+        <v>DefInjected\JobDef\JobDef.xml</v>
       </c>
       <c r="J78" s="41" t="str">
         <f t="shared" si="6"/>
-        <v>PrisonLabor_SupervisePrisonLabor.label</v>
+        <v>PrisonLabor_Mine_Tweak.reportString</v>
       </c>
       <c r="K78" s="47" t="str">
         <f t="shared" si="7"/>
@@ -4353,9 +4393,11 @@
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A79" s="9"/>
+      <c r="A79" s="9" t="s">
+        <v>105</v>
+      </c>
       <c r="B79" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C79" s="34"/>
       <c r="D79" s="12" t="s">
@@ -4365,15 +4407,15 @@
       <c r="F79" s="11"/>
       <c r="G79" s="11"/>
       <c r="H79" s="13" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="I79" s="44" t="str">
-        <f t="shared" si="8"/>
-        <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
+        <f>H$75</f>
+        <v>DefInjected\JobDef\JobDef.xml</v>
       </c>
       <c r="J79" s="41" t="str">
         <f t="shared" si="6"/>
-        <v>PrisonLabor_SupervisePrisonLabor.verb</v>
+        <v>PrisonLabor_Harvest_Tweak.reportString</v>
       </c>
       <c r="K79" s="47" t="str">
         <f t="shared" si="7"/>
@@ -4383,12 +4425,14 @@
         <v>214</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A80" s="9"/>
-      <c r="B80" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C80" s="34"/>
+    <row r="80" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C80" s="35"/>
       <c r="D80" s="12" t="s">
         <v>214</v>
       </c>
@@ -4396,15 +4440,15 @@
       <c r="F80" s="11"/>
       <c r="G80" s="11"/>
       <c r="H80" s="13" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="I80" s="44" t="str">
-        <f t="shared" si="8"/>
-        <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
+        <f>H$75</f>
+        <v>DefInjected\JobDef\JobDef.xml</v>
       </c>
       <c r="J80" s="41" t="str">
         <f t="shared" si="6"/>
-        <v>PrisonLabor_SupervisePrisonLabor.gerund</v>
+        <v>PrisonLabor_CutPlant_Tweak.reportString</v>
       </c>
       <c r="K80" s="47" t="str">
         <f t="shared" si="7"/>
@@ -4414,47 +4458,34 @@
         <v>214</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A81" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C81" s="34"/>
+    <row r="81" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="B81" s="55"/>
+      <c r="C81" s="55"/>
       <c r="D81" s="12" t="s">
         <v>214</v>
       </c>
       <c r="E81" s="11"/>
       <c r="F81" s="11"/>
       <c r="G81" s="11"/>
-      <c r="H81" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="I81" s="44" t="str">
-        <f t="shared" si="8"/>
-        <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
-      </c>
-      <c r="J81" s="41" t="str">
-        <f t="shared" si="6"/>
-        <v>PrisonLabor_DeliverFoodToPrisoner_Tweak.label</v>
-      </c>
-      <c r="K81" s="47" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
+      <c r="H81" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="I81" s="42"/>
+      <c r="J81" s="43"/>
+      <c r="K81" s="48"/>
       <c r="L81" s="20" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A82" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C82" s="34"/>
+      <c r="A82" s="8"/>
+      <c r="B82" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C82" s="33"/>
       <c r="D82" s="12" t="s">
         <v>214</v>
       </c>
@@ -4462,15 +4493,15 @@
       <c r="F82" s="11"/>
       <c r="G82" s="11"/>
       <c r="H82" s="13" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="I82" s="44" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="I82:I102" si="8">H$81</f>
         <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
       </c>
       <c r="J82" s="41" t="str">
         <f t="shared" si="6"/>
-        <v>PrisonLabor_DeliverFoodToPrisoner_Tweak.verb</v>
+        <v>PrisonLabor_SupervisePrisonLabor.label</v>
       </c>
       <c r="K82" s="47" t="str">
         <f t="shared" si="7"/>
@@ -4481,11 +4512,9 @@
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A83" s="9" t="s">
-        <v>105</v>
-      </c>
+      <c r="A83" s="9"/>
       <c r="B83" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C83" s="34"/>
       <c r="D83" s="12" t="s">
@@ -4495,7 +4524,7 @@
       <c r="F83" s="11"/>
       <c r="G83" s="11"/>
       <c r="H83" s="13" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="I83" s="44" t="str">
         <f t="shared" si="8"/>
@@ -4503,7 +4532,7 @@
       </c>
       <c r="J83" s="41" t="str">
         <f t="shared" si="6"/>
-        <v>PrisonLabor_DeliverFoodToPrisoner_Tweak.gerund</v>
+        <v>PrisonLabor_SupervisePrisonLabor.verb</v>
       </c>
       <c r="K83" s="47" t="str">
         <f t="shared" si="7"/>
@@ -4514,11 +4543,9 @@
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A84" s="9" t="s">
-        <v>105</v>
-      </c>
+      <c r="A84" s="9"/>
       <c r="B84" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C84" s="34"/>
       <c r="D84" s="12" t="s">
@@ -4528,7 +4555,7 @@
       <c r="F84" s="11"/>
       <c r="G84" s="11"/>
       <c r="H84" s="13" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="I84" s="44" t="str">
         <f t="shared" si="8"/>
@@ -4536,7 +4563,7 @@
       </c>
       <c r="J84" s="41" t="str">
         <f t="shared" si="6"/>
-        <v>PrisonLabor_Mine_Tweak.label</v>
+        <v>PrisonLabor_SupervisePrisonLabor.gerund</v>
       </c>
       <c r="K84" s="47" t="str">
         <f t="shared" si="7"/>
@@ -4551,7 +4578,7 @@
         <v>105</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C85" s="34"/>
       <c r="D85" s="12" t="s">
@@ -4561,7 +4588,7 @@
       <c r="F85" s="11"/>
       <c r="G85" s="11"/>
       <c r="H85" s="13" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="I85" s="44" t="str">
         <f t="shared" si="8"/>
@@ -4569,7 +4596,7 @@
       </c>
       <c r="J85" s="41" t="str">
         <f t="shared" si="6"/>
-        <v>PrisonLabor_Mine_Tweak.verb</v>
+        <v>PrisonLabor_DeliverFoodToPrisoner_Tweak.label</v>
       </c>
       <c r="K85" s="47" t="str">
         <f t="shared" si="7"/>
@@ -4584,7 +4611,7 @@
         <v>105</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C86" s="34"/>
       <c r="D86" s="12" t="s">
@@ -4594,7 +4621,7 @@
       <c r="F86" s="11"/>
       <c r="G86" s="11"/>
       <c r="H86" s="13" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="I86" s="44" t="str">
         <f t="shared" si="8"/>
@@ -4602,7 +4629,7 @@
       </c>
       <c r="J86" s="41" t="str">
         <f t="shared" si="6"/>
-        <v>PrisonLabor_Mine_Tweak.gerund</v>
+        <v>PrisonLabor_DeliverFoodToPrisoner_Tweak.verb</v>
       </c>
       <c r="K86" s="47" t="str">
         <f t="shared" si="7"/>
@@ -4617,7 +4644,7 @@
         <v>105</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C87" s="34"/>
       <c r="D87" s="12" t="s">
@@ -4627,7 +4654,7 @@
       <c r="F87" s="11"/>
       <c r="G87" s="11"/>
       <c r="H87" s="13" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="I87" s="44" t="str">
         <f t="shared" si="8"/>
@@ -4635,7 +4662,7 @@
       </c>
       <c r="J87" s="41" t="str">
         <f t="shared" si="6"/>
-        <v>PrisonLabor_PlantsCut_Tweak.label</v>
+        <v>PrisonLabor_DeliverFoodToPrisoner_Tweak.gerund</v>
       </c>
       <c r="K87" s="47" t="str">
         <f t="shared" si="7"/>
@@ -4650,7 +4677,7 @@
         <v>105</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C88" s="34"/>
       <c r="D88" s="12" t="s">
@@ -4660,7 +4687,7 @@
       <c r="F88" s="11"/>
       <c r="G88" s="11"/>
       <c r="H88" s="13" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="I88" s="44" t="str">
         <f t="shared" si="8"/>
@@ -4668,7 +4695,7 @@
       </c>
       <c r="J88" s="41" t="str">
         <f t="shared" si="6"/>
-        <v>PrisonLabor_PlantsCut_Tweak.verb</v>
+        <v>PrisonLabor_Mine_Tweak.label</v>
       </c>
       <c r="K88" s="47" t="str">
         <f t="shared" si="7"/>
@@ -4683,7 +4710,7 @@
         <v>105</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C89" s="34"/>
       <c r="D89" s="12" t="s">
@@ -4693,7 +4720,7 @@
       <c r="F89" s="11"/>
       <c r="G89" s="11"/>
       <c r="H89" s="13" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="I89" s="44" t="str">
         <f t="shared" si="8"/>
@@ -4701,7 +4728,7 @@
       </c>
       <c r="J89" s="41" t="str">
         <f t="shared" si="6"/>
-        <v>PrisonLabor_PlantsCut_Tweak.gerund</v>
+        <v>PrisonLabor_Mine_Tweak.verb</v>
       </c>
       <c r="K89" s="47" t="str">
         <f t="shared" si="7"/>
@@ -4716,7 +4743,7 @@
         <v>105</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C90" s="34"/>
       <c r="D90" s="12" t="s">
@@ -4726,7 +4753,7 @@
       <c r="F90" s="11"/>
       <c r="G90" s="11"/>
       <c r="H90" s="13" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="I90" s="44" t="str">
         <f t="shared" si="8"/>
@@ -4734,7 +4761,7 @@
       </c>
       <c r="J90" s="41" t="str">
         <f t="shared" si="6"/>
-        <v>PrisonLabor_GrowerHarvest_Tweak.label</v>
+        <v>PrisonLabor_Mine_Tweak.gerund</v>
       </c>
       <c r="K90" s="47" t="str">
         <f t="shared" si="7"/>
@@ -4749,7 +4776,7 @@
         <v>105</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C91" s="34"/>
       <c r="D91" s="12" t="s">
@@ -4759,7 +4786,7 @@
       <c r="F91" s="11"/>
       <c r="G91" s="11"/>
       <c r="H91" s="13" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="I91" s="44" t="str">
         <f t="shared" si="8"/>
@@ -4767,7 +4794,7 @@
       </c>
       <c r="J91" s="41" t="str">
         <f t="shared" si="6"/>
-        <v>PrisonLabor_GrowerHarvest_Tweak.verb</v>
+        <v>PrisonLabor_PlantsCut_Tweak.label</v>
       </c>
       <c r="K91" s="47" t="str">
         <f t="shared" si="7"/>
@@ -4782,7 +4809,7 @@
         <v>105</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C92" s="34"/>
       <c r="D92" s="12" t="s">
@@ -4792,7 +4819,7 @@
       <c r="F92" s="11"/>
       <c r="G92" s="11"/>
       <c r="H92" s="13" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="I92" s="44" t="str">
         <f t="shared" si="8"/>
@@ -4800,7 +4827,7 @@
       </c>
       <c r="J92" s="41" t="str">
         <f t="shared" si="6"/>
-        <v>PrisonLabor_GrowerHarvest_Tweak.gerund</v>
+        <v>PrisonLabor_PlantsCut_Tweak.verb</v>
       </c>
       <c r="K92" s="47" t="str">
         <f t="shared" si="7"/>
@@ -4815,7 +4842,7 @@
         <v>105</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C93" s="34"/>
       <c r="D93" s="12" t="s">
@@ -4825,7 +4852,7 @@
       <c r="F93" s="11"/>
       <c r="G93" s="11"/>
       <c r="H93" s="13" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="I93" s="44" t="str">
         <f t="shared" si="8"/>
@@ -4833,7 +4860,7 @@
       </c>
       <c r="J93" s="41" t="str">
         <f t="shared" si="6"/>
-        <v>PrisonLabor_GrowerSow_Tweak.label</v>
+        <v>PrisonLabor_PlantsCut_Tweak.gerund</v>
       </c>
       <c r="K93" s="47" t="str">
         <f t="shared" si="7"/>
@@ -4848,7 +4875,7 @@
         <v>105</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C94" s="34"/>
       <c r="D94" s="12" t="s">
@@ -4858,7 +4885,7 @@
       <c r="F94" s="11"/>
       <c r="G94" s="11"/>
       <c r="H94" s="13" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="I94" s="44" t="str">
         <f t="shared" si="8"/>
@@ -4866,7 +4893,7 @@
       </c>
       <c r="J94" s="41" t="str">
         <f t="shared" si="6"/>
-        <v>PrisonLabor_GrowerSow_Tweak.verb</v>
+        <v>PrisonLabor_GrowerHarvest_Tweak.label</v>
       </c>
       <c r="K94" s="47" t="str">
         <f t="shared" si="7"/>
@@ -4881,7 +4908,7 @@
         <v>105</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C95" s="34"/>
       <c r="D95" s="12" t="s">
@@ -4891,7 +4918,7 @@
       <c r="F95" s="11"/>
       <c r="G95" s="11"/>
       <c r="H95" s="13" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="I95" s="44" t="str">
         <f t="shared" si="8"/>
@@ -4899,7 +4926,7 @@
       </c>
       <c r="J95" s="41" t="str">
         <f t="shared" si="6"/>
-        <v>PrisonLabor_GrowerSow_Tweak.gerund</v>
+        <v>PrisonLabor_GrowerHarvest_Tweak.verb</v>
       </c>
       <c r="K95" s="47" t="str">
         <f t="shared" si="7"/>
@@ -4914,7 +4941,7 @@
         <v>105</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C96" s="34"/>
       <c r="D96" s="12" t="s">
@@ -4924,7 +4951,7 @@
       <c r="F96" s="11"/>
       <c r="G96" s="11"/>
       <c r="H96" s="13" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="I96" s="44" t="str">
         <f t="shared" si="8"/>
@@ -4932,7 +4959,7 @@
       </c>
       <c r="J96" s="41" t="str">
         <f t="shared" si="6"/>
-        <v>PrisonLabor_CleanFilth_Tweak.label</v>
+        <v>PrisonLabor_GrowerHarvest_Tweak.gerund</v>
       </c>
       <c r="K96" s="47" t="str">
         <f t="shared" si="7"/>
@@ -4947,7 +4974,7 @@
         <v>105</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C97" s="34"/>
       <c r="D97" s="12" t="s">
@@ -4957,7 +4984,7 @@
       <c r="F97" s="11"/>
       <c r="G97" s="11"/>
       <c r="H97" s="13" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="I97" s="44" t="str">
         <f t="shared" si="8"/>
@@ -4965,7 +4992,7 @@
       </c>
       <c r="J97" s="41" t="str">
         <f t="shared" si="6"/>
-        <v>PrisonLabor_CleanFilth_Tweak.verb</v>
+        <v>PrisonLabor_GrowerSow_Tweak.label</v>
       </c>
       <c r="K97" s="47" t="str">
         <f t="shared" si="7"/>
@@ -4975,14 +5002,14 @@
         <v>214</v>
       </c>
     </row>
-    <row r="98" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="10" t="s">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A98" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B98" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C98" s="35"/>
+      <c r="B98" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C98" s="34"/>
       <c r="D98" s="12" t="s">
         <v>214</v>
       </c>
@@ -4990,7 +5017,7 @@
       <c r="F98" s="11"/>
       <c r="G98" s="11"/>
       <c r="H98" s="13" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="I98" s="44" t="str">
         <f t="shared" si="8"/>
@@ -4998,7 +5025,7 @@
       </c>
       <c r="J98" s="41" t="str">
         <f t="shared" si="6"/>
-        <v>PrisonLabor_CleanFilth_Tweak.gerund</v>
+        <v>PrisonLabor_GrowerSow_Tweak.verb</v>
       </c>
       <c r="K98" s="47" t="str">
         <f t="shared" si="7"/>
@@ -5008,53 +5035,63 @@
         <v>214</v>
       </c>
     </row>
-    <row r="99" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="57" t="s">
-        <v>208</v>
-      </c>
-      <c r="B99" s="58"/>
-      <c r="C99" s="59"/>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A99" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C99" s="34"/>
       <c r="D99" s="12" t="s">
         <v>214</v>
       </c>
       <c r="E99" s="11"/>
       <c r="F99" s="11"/>
       <c r="G99" s="11"/>
-      <c r="H99" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="I99" s="42"/>
-      <c r="J99" s="43"/>
-      <c r="K99" s="48"/>
+      <c r="H99" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="I99" s="44" t="str">
+        <f t="shared" si="8"/>
+        <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
+      </c>
+      <c r="J99" s="41" t="str">
+        <f t="shared" si="6"/>
+        <v>PrisonLabor_GrowerSow_Tweak.gerund</v>
+      </c>
+      <c r="K99" s="47" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="L99" s="20" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A100" s="8"/>
-      <c r="B100" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C100" s="33" t="str">
-        <f>C3&amp;""</f>
-        <v/>
-      </c>
+      <c r="A100" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C100" s="34"/>
       <c r="D100" s="12" t="s">
         <v>214</v>
       </c>
       <c r="E100" s="11"/>
       <c r="F100" s="11"/>
       <c r="G100" s="11"/>
-      <c r="H100" s="17" t="s">
-        <v>209</v>
+      <c r="H100" s="13" t="s">
+        <v>201</v>
       </c>
       <c r="I100" s="44" t="str">
-        <f>H$99</f>
-        <v>DefInjected\InteractionDefs\PrisonerInteractionModeDef.xml</v>
+        <f t="shared" si="8"/>
+        <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
       </c>
       <c r="J100" s="41" t="str">
         <f t="shared" si="6"/>
-        <v>PrisonLabor_workOption.label</v>
+        <v>PrisonLabor_CleanFilth_Tweak.label</v>
       </c>
       <c r="K100" s="47" t="str">
         <f t="shared" si="7"/>
@@ -5064,31 +5101,30 @@
         <v>214</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="18"/>
-      <c r="B101" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C101" s="36" t="str">
-        <f>C4&amp;""</f>
-        <v/>
-      </c>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A101" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C101" s="34"/>
       <c r="D101" s="12" t="s">
         <v>214</v>
       </c>
       <c r="E101" s="11"/>
       <c r="F101" s="11"/>
       <c r="G101" s="11"/>
-      <c r="H101" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="I101" s="45" t="str">
-        <f>H$99</f>
-        <v>DefInjected\InteractionDefs\PrisonerInteractionModeDef.xml</v>
-      </c>
-      <c r="J101" s="46" t="str">
+      <c r="H101" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="I101" s="44" t="str">
+        <f t="shared" si="8"/>
+        <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
+      </c>
+      <c r="J101" s="41" t="str">
         <f t="shared" si="6"/>
-        <v>PrisonLabor_workAndRecruitOption.label</v>
+        <v>PrisonLabor_CleanFilth_Tweak.verb</v>
       </c>
       <c r="K101" s="47" t="str">
         <f t="shared" si="7"/>
@@ -5098,24 +5134,32 @@
         <v>214</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="55" t="s">
-        <v>95</v>
-      </c>
-      <c r="B102" s="55"/>
-      <c r="C102" s="55"/>
+    <row r="102" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C102" s="35"/>
       <c r="D102" s="12" t="s">
         <v>214</v>
       </c>
       <c r="E102" s="11"/>
       <c r="F102" s="11"/>
       <c r="G102" s="11"/>
-      <c r="H102" s="23"/>
-      <c r="I102" s="30" t="s">
-        <v>159</v>
-      </c>
-      <c r="J102" s="30"/>
-      <c r="K102" s="31" t="str">
+      <c r="H102" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="I102" s="44" t="str">
+        <f t="shared" si="8"/>
+        <v>DefInjected\WorkGiverDef\WorkGiverDef.xml</v>
+      </c>
+      <c r="J102" s="41" t="str">
+        <f t="shared" si="6"/>
+        <v>PrisonLabor_CleanFilth_Tweak.gerund</v>
+      </c>
+      <c r="K102" s="47" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
@@ -5123,157 +5167,230 @@
         <v>214</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A103" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="B103" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C103" s="33"/>
+    <row r="103" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="57" t="s">
+        <v>208</v>
+      </c>
+      <c r="B103" s="58"/>
+      <c r="C103" s="59"/>
       <c r="D103" s="12" t="s">
         <v>214</v>
       </c>
       <c r="E103" s="11"/>
       <c r="F103" s="11"/>
       <c r="G103" s="11"/>
-      <c r="H103" s="13"/>
-      <c r="I103" s="27"/>
-      <c r="J103" s="27"/>
-      <c r="K103" s="28"/>
+      <c r="H103" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="I103" s="42"/>
+      <c r="J103" s="43"/>
+      <c r="K103" s="48"/>
       <c r="L103" s="20" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="270" x14ac:dyDescent="0.25">
-      <c r="A104" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C104" s="34"/>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A104" s="8"/>
+      <c r="B104" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C104" s="33" t="str">
+        <f>C3&amp;""</f>
+        <v/>
+      </c>
       <c r="D104" s="12" t="s">
         <v>214</v>
       </c>
       <c r="E104" s="11"/>
       <c r="F104" s="11"/>
       <c r="G104" s="11"/>
-      <c r="H104" s="13"/>
-      <c r="I104" s="27"/>
-      <c r="J104" s="27"/>
-      <c r="K104" s="28"/>
+      <c r="H104" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="I104" s="44" t="str">
+        <f>H$103</f>
+        <v>DefInjected\InteractionDefs\PrisonerInteractionModeDef.xml</v>
+      </c>
+      <c r="J104" s="41" t="str">
+        <f t="shared" si="6"/>
+        <v>PrisonLabor_workOption.label</v>
+      </c>
+      <c r="K104" s="47" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="L104" s="20" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="105" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A105" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C105" s="34"/>
+    <row r="105" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="18"/>
+      <c r="B105" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C105" s="36" t="str">
+        <f>C4&amp;""</f>
+        <v/>
+      </c>
       <c r="D105" s="12" t="s">
         <v>214</v>
       </c>
       <c r="E105" s="11"/>
       <c r="F105" s="11"/>
       <c r="G105" s="11"/>
-      <c r="H105" s="13"/>
-      <c r="I105" s="27"/>
-      <c r="J105" s="27"/>
-      <c r="K105" s="28"/>
+      <c r="H105" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="I105" s="45" t="str">
+        <f>H$103</f>
+        <v>DefInjected\InteractionDefs\PrisonerInteractionModeDef.xml</v>
+      </c>
+      <c r="J105" s="46" t="str">
+        <f t="shared" si="6"/>
+        <v>PrisonLabor_workAndRecruitOption.label</v>
+      </c>
+      <c r="K105" s="47" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="L105" s="20" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A106" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C106" s="34"/>
+    <row r="106" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="55" t="s">
+        <v>95</v>
+      </c>
+      <c r="B106" s="55"/>
+      <c r="C106" s="55"/>
       <c r="D106" s="12" t="s">
         <v>214</v>
       </c>
       <c r="E106" s="11"/>
       <c r="F106" s="11"/>
       <c r="G106" s="11"/>
-      <c r="H106" s="13"/>
-      <c r="I106" s="27"/>
-      <c r="J106" s="27"/>
-      <c r="K106" s="28"/>
+      <c r="H106" s="23"/>
+      <c r="I106" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="J106" s="30"/>
+      <c r="K106" s="31" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="L106" s="20" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="107" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A107" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C107" s="34"/>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A107" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C107" s="33"/>
       <c r="D107" s="12" t="s">
         <v>214</v>
       </c>
       <c r="E107" s="11"/>
       <c r="F107" s="11"/>
       <c r="G107" s="11"/>
-      <c r="H107" s="14"/>
-      <c r="I107" s="29"/>
-      <c r="J107" s="29"/>
-      <c r="K107" s="26"/>
+      <c r="H107" s="13"/>
+      <c r="I107" s="27"/>
+      <c r="J107" s="27"/>
+      <c r="K107" s="28"/>
       <c r="L107" s="20" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" ht="270" x14ac:dyDescent="0.25">
+      <c r="A108" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C108" s="34"/>
       <c r="D108" s="12" t="s">
         <v>214</v>
       </c>
       <c r="E108" s="11"/>
       <c r="F108" s="11"/>
       <c r="G108" s="11"/>
-      <c r="H108" s="11"/>
-      <c r="I108" s="24"/>
-      <c r="J108" s="24"/>
-      <c r="K108" s="24"/>
-      <c r="L108" s="11"/>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H108" s="13"/>
+      <c r="I108" s="27"/>
+      <c r="J108" s="27"/>
+      <c r="K108" s="28"/>
+      <c r="L108" s="20" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A109" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C109" s="34"/>
       <c r="D109" s="12" t="s">
         <v>214</v>
       </c>
       <c r="E109" s="11"/>
       <c r="F109" s="11"/>
       <c r="G109" s="11"/>
-      <c r="H109" s="11"/>
-      <c r="K109" s="24"/>
-      <c r="L109" s="11"/>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H109" s="13"/>
+      <c r="I109" s="27"/>
+      <c r="J109" s="27"/>
+      <c r="K109" s="28"/>
+      <c r="L109" s="20" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A110" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C110" s="34"/>
       <c r="D110" s="12" t="s">
         <v>214</v>
       </c>
       <c r="E110" s="11"/>
       <c r="F110" s="11"/>
       <c r="G110" s="11"/>
-      <c r="H110" s="11"/>
-    </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H110" s="13"/>
+      <c r="I110" s="27"/>
+      <c r="J110" s="27"/>
+      <c r="K110" s="28"/>
+      <c r="L110" s="20" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A111" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C111" s="34"/>
       <c r="D111" s="12" t="s">
         <v>214</v>
       </c>
       <c r="E111" s="11"/>
       <c r="F111" s="11"/>
       <c r="G111" s="11"/>
-      <c r="H111" s="11"/>
+      <c r="H111" s="14"/>
+      <c r="I111" s="29"/>
+      <c r="J111" s="29"/>
+      <c r="K111" s="26"/>
+      <c r="L111" s="20" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D112" s="12" t="s">
@@ -5283,8 +5400,12 @@
       <c r="F112" s="11"/>
       <c r="G112" s="11"/>
       <c r="H112" s="11"/>
-    </row>
-    <row r="113" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="I112" s="24"/>
+      <c r="J112" s="24"/>
+      <c r="K112" s="24"/>
+      <c r="L112" s="11"/>
+    </row>
+    <row r="113" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D113" s="12" t="s">
         <v>214</v>
       </c>
@@ -5292,8 +5413,10 @@
       <c r="F113" s="11"/>
       <c r="G113" s="11"/>
       <c r="H113" s="11"/>
-    </row>
-    <row r="114" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="K113" s="24"/>
+      <c r="L113" s="11"/>
+    </row>
+    <row r="114" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D114" s="12" t="s">
         <v>214</v>
       </c>
@@ -5302,7 +5425,7 @@
       <c r="G114" s="11"/>
       <c r="H114" s="11"/>
     </row>
-    <row r="115" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D115" s="12" t="s">
         <v>214</v>
       </c>
@@ -5311,7 +5434,7 @@
       <c r="G115" s="11"/>
       <c r="H115" s="11"/>
     </row>
-    <row r="116" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D116" s="12" t="s">
         <v>214</v>
       </c>
@@ -5320,7 +5443,7 @@
       <c r="G116" s="11"/>
       <c r="H116" s="11"/>
     </row>
-    <row r="117" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D117" s="12" t="s">
         <v>214</v>
       </c>
@@ -5329,7 +5452,7 @@
       <c r="G117" s="11"/>
       <c r="H117" s="11"/>
     </row>
-    <row r="118" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D118" s="12" t="s">
         <v>214</v>
       </c>
@@ -5338,7 +5461,7 @@
       <c r="G118" s="11"/>
       <c r="H118" s="11"/>
     </row>
-    <row r="119" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D119" s="12" t="s">
         <v>214</v>
       </c>
@@ -5347,7 +5470,7 @@
       <c r="G119" s="11"/>
       <c r="H119" s="11"/>
     </row>
-    <row r="120" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D120" s="12" t="s">
         <v>214</v>
       </c>
@@ -5356,7 +5479,7 @@
       <c r="G120" s="11"/>
       <c r="H120" s="11"/>
     </row>
-    <row r="121" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D121" s="12" t="s">
         <v>214</v>
       </c>
@@ -5365,7 +5488,7 @@
       <c r="G121" s="11"/>
       <c r="H121" s="11"/>
     </row>
-    <row r="122" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D122" s="12" t="s">
         <v>214</v>
       </c>
@@ -5374,7 +5497,7 @@
       <c r="G122" s="11"/>
       <c r="H122" s="11"/>
     </row>
-    <row r="123" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D123" s="12" t="s">
         <v>214</v>
       </c>
@@ -5383,7 +5506,7 @@
       <c r="G123" s="11"/>
       <c r="H123" s="11"/>
     </row>
-    <row r="124" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D124" s="12" t="s">
         <v>214</v>
       </c>
@@ -5392,7 +5515,7 @@
       <c r="G124" s="11"/>
       <c r="H124" s="11"/>
     </row>
-    <row r="125" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D125" s="12" t="s">
         <v>214</v>
       </c>
@@ -5401,7 +5524,7 @@
       <c r="G125" s="11"/>
       <c r="H125" s="11"/>
     </row>
-    <row r="126" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D126" s="12" t="s">
         <v>214</v>
       </c>
@@ -5410,7 +5533,7 @@
       <c r="G126" s="11"/>
       <c r="H126" s="11"/>
     </row>
-    <row r="127" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D127" s="12" t="s">
         <v>214</v>
       </c>
@@ -5419,7 +5542,7 @@
       <c r="G127" s="11"/>
       <c r="H127" s="11"/>
     </row>
-    <row r="128" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D128" s="12" t="s">
         <v>214</v>
       </c>
@@ -5456,28 +5579,36 @@
       <c r="H131" s="11"/>
     </row>
     <row r="132" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D132" s="11"/>
+      <c r="D132" s="12" t="s">
+        <v>214</v>
+      </c>
       <c r="E132" s="11"/>
       <c r="F132" s="11"/>
       <c r="G132" s="11"/>
       <c r="H132" s="11"/>
     </row>
     <row r="133" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D133" s="11"/>
+      <c r="D133" s="12" t="s">
+        <v>214</v>
+      </c>
       <c r="E133" s="11"/>
       <c r="F133" s="11"/>
       <c r="G133" s="11"/>
       <c r="H133" s="11"/>
     </row>
     <row r="134" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D134" s="11"/>
+      <c r="D134" s="12" t="s">
+        <v>214</v>
+      </c>
       <c r="E134" s="11"/>
       <c r="F134" s="11"/>
       <c r="G134" s="11"/>
       <c r="H134" s="11"/>
     </row>
     <row r="135" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D135" s="11"/>
+      <c r="D135" s="12" t="s">
+        <v>214</v>
+      </c>
       <c r="E135" s="11"/>
       <c r="F135" s="11"/>
       <c r="G135" s="11"/>
@@ -5666,15 +5797,31 @@
       <c r="H161" s="11"/>
     </row>
     <row r="162" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D162" s="11"/>
+      <c r="E162" s="11"/>
+      <c r="F162" s="11"/>
+      <c r="G162" s="11"/>
       <c r="H162" s="11"/>
     </row>
     <row r="163" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D163" s="11"/>
+      <c r="E163" s="11"/>
+      <c r="F163" s="11"/>
+      <c r="G163" s="11"/>
       <c r="H163" s="11"/>
     </row>
     <row r="164" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D164" s="11"/>
+      <c r="E164" s="11"/>
+      <c r="F164" s="11"/>
+      <c r="G164" s="11"/>
       <c r="H164" s="11"/>
     </row>
     <row r="165" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D165" s="11"/>
+      <c r="E165" s="11"/>
+      <c r="F165" s="11"/>
+      <c r="G165" s="11"/>
       <c r="H165" s="11"/>
     </row>
     <row r="166" spans="4:8" x14ac:dyDescent="0.25">
@@ -6144,20 +6291,32 @@
     </row>
     <row r="321" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H321" s="11"/>
+    </row>
+    <row r="322" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H322" s="11"/>
+    </row>
+    <row r="323" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H323" s="11"/>
+    </row>
+    <row r="324" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H324" s="11"/>
+    </row>
+    <row r="325" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H325" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="H1:K1"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A77:C77"/>
-    <mergeCell ref="A102:C102"/>
+    <mergeCell ref="A81:C81"/>
+    <mergeCell ref="A106:C106"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="A66:C66"/>
     <mergeCell ref="A71:C71"/>
-    <mergeCell ref="A99:C99"/>
+    <mergeCell ref="A75:C75"/>
+    <mergeCell ref="A103:C103"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>